<commit_message>
Update. Adding Hadi's survey.
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hadisharifi/Documents/CSE6242/Project/proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAE6835-6AB0-5C49-A84A-608B170D2C7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45BB2B0-C1AB-AA41-99FA-65A50248BC25}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22180" yWindow="-19240" windowWidth="35120" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4920,7 +4920,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="landscape" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Latest update. 1194 words.
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hadisharifi/Documents/CSE6242/Project/proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45BB2B0-C1AB-AA41-99FA-65A50248BC25}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F00488-7B94-5646-8345-ED483B2AECD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22180" yWindow="-19240" windowWidth="35120" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16860" yWindow="-20600" windowWidth="35120" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <t>Social Media</t>
   </si>
   <si>
-    <t>Gaming/Technology</t>
-  </si>
-  <si>
     <t>Physical Activity</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>Lieteratur Review on Relationship between Six Habit Factors and Anxiety/Depression</t>
+  </si>
+  <si>
+    <t>Technology/Education</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1649,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1"/>
@@ -1670,7 +1670,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1686,7 +1686,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2" s="47" t="s">
         <v>17</v>
@@ -2500,7 +2500,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="52"/>
       <c r="D8" s="16"/>
@@ -2593,7 +2593,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="58">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="59">
         <f>Project_Start</f>
@@ -2684,13 +2684,13 @@
         <v>36</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="57" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="58">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E10" s="59">
         <f>Project_Start</f>
@@ -2785,7 +2785,7 @@
         <v>40</v>
       </c>
       <c r="D11" s="58">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="59">
         <f>Project_Start</f>
@@ -2874,13 +2874,13 @@
     <row r="12" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A12" s="44"/>
       <c r="B12" s="56" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C12" s="57" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="58">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E12" s="59">
         <f>Project_Start</f>
@@ -2969,13 +2969,13 @@
     <row r="13" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="44"/>
       <c r="B13" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="57" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="58">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="59">
         <f>Project_Start</f>
@@ -3066,7 +3066,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="53"/>
       <c r="D14" s="19"/>
@@ -3151,13 +3151,13 @@
     <row r="15" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A15" s="45"/>
       <c r="B15" s="64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="66">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="67">
         <f>E13+6</f>
@@ -3246,10 +3246,10 @@
     <row r="16" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A16" s="44"/>
       <c r="B16" s="64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="66">
         <v>0</v>
@@ -3343,7 +3343,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="69"/>
       <c r="D17" s="70"/>
@@ -3523,7 +3523,7 @@
     <row r="19" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A19" s="44"/>
       <c r="B19" s="73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="74" t="s">
         <v>39</v>
@@ -3713,7 +3713,7 @@
     <row r="21" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A21" s="44"/>
       <c r="B21" s="73" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C21" s="74" t="s">
         <v>41</v>
@@ -3808,7 +3808,7 @@
     <row r="22" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A22" s="44"/>
       <c r="B22" s="73" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="74" t="s">
         <v>42</v>
@@ -3900,10 +3900,10 @@
     <row r="23" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A23" s="44"/>
       <c r="B23" s="73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="74" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" s="75">
         <v>0</v>
@@ -3992,7 +3992,7 @@
     <row r="24" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A24" s="44"/>
       <c r="B24" s="73" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="74" t="s">
         <v>38</v>
@@ -4086,7 +4086,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="77" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="78"/>
       <c r="D25" s="79"/>
@@ -4171,10 +4171,10 @@
     <row r="26" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A26" s="44"/>
       <c r="B26" s="82" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="84">
         <v>0</v>
@@ -4266,10 +4266,10 @@
     <row r="27" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A27" s="44"/>
       <c r="B27" s="82" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="84">
         <v>0</v>
@@ -4361,10 +4361,10 @@
     <row r="28" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A28" s="44"/>
       <c r="B28" s="82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="84">
         <v>0</v>
@@ -4456,10 +4456,10 @@
     <row r="29" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A29" s="44"/>
       <c r="B29" s="82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="84">
         <v>0</v>
@@ -4551,10 +4551,10 @@
     <row r="30" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A30" s="44"/>
       <c r="B30" s="82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="84">
         <v>0</v>

</xml_diff>